<commit_message>
basic salary upload done
</commit_message>
<xml_diff>
--- a/excelforms/basicsalary.xlsx
+++ b/excelforms/basicsalary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\payroll\excelforms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBC98ED-E5BA-493D-9AF2-D5CACB660087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D707E8D2-F276-4CF5-9FFC-121CD19FD684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,16 +83,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -113,8 +117,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E18AD355-88EB-46C2-A57C-A710F528C13F}" name="رقم القيد"/>
     <tableColumn id="2" xr3:uid="{6123294E-83E4-4232-9ADB-4F0873F170E2}" name="الاسم"/>
-    <tableColumn id="3" xr3:uid="{9E062A66-EB9E-4833-821A-4607D845A9F4}" name="الاجر الاساسى"/>
-    <tableColumn id="4" xr3:uid="{F2E4ED7C-17EF-4D2F-9B80-651A45868C8A}" name="التاريخ" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{9E062A66-EB9E-4833-821A-4607D845A9F4}" name="الاجر الاساسى" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{F2E4ED7C-17EF-4D2F-9B80-651A45868C8A}" name="التاريخ" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -386,7 +390,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +419,7 @@
       <c r="A2">
         <v>1152</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>30</v>
       </c>
       <c r="D2" s="1">
@@ -426,7 +430,7 @@
       <c r="A3">
         <v>167</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>30</v>
       </c>
       <c r="D3" s="1">
@@ -437,7 +441,7 @@
       <c r="A4">
         <v>900</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>30</v>
       </c>
       <c r="D4" s="1">

</xml_diff>